<commit_message>
working hours adjusted and design slightly modified
</commit_message>
<xml_diff>
--- a/indinf02-working-hourse-janeczek-mair.xlsx
+++ b/indinf02-working-hourse-janeczek-mair.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>PHASE</t>
   </si>
@@ -68,7 +68,16 @@
     <t>Writing the struct of the protocol</t>
   </si>
   <si>
-    <t>skill comes with practice</t>
+    <t>Preperation</t>
+  </si>
+  <si>
+    <t>Configuration of the Hardware Environment</t>
+  </si>
+  <si>
+    <t>Skill comes with practice</t>
+  </si>
+  <si>
+    <t>I had some issues finding an improving an existing Makefile, preparing the whole hardware environment(flashing tool, linker, compiler, etc.) and actually testing the whole process by successfully flashing a working program onto the TM4C123GXL</t>
   </si>
 </sst>
 </file>
@@ -76,9 +85,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -110,8 +119,22 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,8 +153,18 @@
         <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -154,11 +187,268 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color theme="8"/>
+      </right>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color theme="8"/>
+      </right>
+      <top style="medium">
+        <color theme="8"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color theme="8"/>
+      </right>
+      <top style="medium">
+        <color theme="8"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right style="medium">
+        <color theme="8"/>
+      </right>
+      <top style="medium">
+        <color theme="8"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color theme="8"/>
+      </right>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right style="medium">
+        <color theme="8"/>
+      </right>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom style="thin">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color theme="8"/>
+      </right>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color theme="8"/>
+      </right>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right style="medium">
+        <color theme="8"/>
+      </right>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF31859C"/>
+      </right>
+      <top style="medium">
+        <color theme="8"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF31859C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF31859C"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF31859C"/>
+      </right>
+      <top style="medium">
+        <color theme="8"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF31859C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF31859C"/>
+      </left>
+      <right style="medium">
+        <color theme="8"/>
+      </right>
+      <top style="medium">
+        <color theme="8"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF31859C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF31859C"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF31859C"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF31859C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF31859C"/>
+      </left>
+      <right style="medium">
+        <color theme="8"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF31859C"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF31859C"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF31859C"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF31859C"/>
+      </top>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF31859C"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF31859C"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF31859C"/>
+      </top>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF31859C"/>
+      </left>
+      <right style="medium">
+        <color theme="8"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF31859C"/>
+      </top>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -169,30 +459,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -200,31 +469,112 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="46" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="46" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="5" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="3" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="46" fontId="3" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="46" fontId="3" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="3" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -595,23 +945,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="35.44140625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="12" style="13" customWidth="1"/>
-    <col min="6" max="6" width="9" style="13" customWidth="1"/>
-    <col min="7" max="7" width="25" style="12" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="12" style="6" customWidth="1"/>
+    <col min="6" max="6" width="9" style="6" customWidth="1"/>
+    <col min="7" max="7" width="70" style="5" customWidth="1"/>
+    <col min="8" max="8" width="0.33203125" customWidth="1"/>
+    <col min="9" max="9" width="0.77734375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -619,17 +971,20 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -637,147 +992,159 @@
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:7" s="13" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="6" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="27" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="5">
+      <c r="B5" s="28">
         <v>41925</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="11">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="12">
         <v>1.113425925925926E-2</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="28">
+        <v>41925</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="12">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0.18717592592592591</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="28"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="29"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="11"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="28"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="29"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="11"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="28"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="29"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="28"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="29"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="28"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="29"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="11"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="28"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="29"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="11"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="28"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="29"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="11"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="28"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="29"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="17">
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="32">
         <f>SUM(E5:E14)</f>
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="F15" s="17">
+        <v>0.125</v>
+      </c>
+      <c r="F15" s="32">
         <f>SUM(F5:F14)</f>
-        <v>1.113425925925926E-2</v>
-      </c>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>0.19831018518518517</v>
+      </c>
+      <c r="G15" s="33"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
@@ -811,8 +1178,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:E2"/>
     <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -821,22 +1188,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.109375"/>
-    <col min="3" max="3" width="15.5546875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="37.6640625" style="13"/>
+    <col min="3" max="3" width="15.5546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="37.6640625" style="6"/>
     <col min="5" max="5" width="14.88671875" customWidth="1"/>
-    <col min="7" max="7" width="23.6640625" customWidth="1"/>
+    <col min="7" max="7" width="42" customWidth="1"/>
+    <col min="8" max="8" width="0.44140625" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -844,153 +1213,159 @@
       <c r="E1" s="3"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="19"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="20"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="19"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="20"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="11"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="19"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="20"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="11"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="19"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="20"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="11"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="19"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="20"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="19"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="20"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="19"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="20"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="11"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="19"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="20"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="11"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="19"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="20"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="11"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="19"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="20"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="17">
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="23">
         <f>SUM(E5:E14)</f>
         <v>0</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="23">
         <f>SUM(F5:F14)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G15" s="24"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
@@ -1024,8 +1399,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:E2"/>
     <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1037,7 +1412,7 @@
   <dimension ref="A3:D8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1047,65 +1422,65 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-    </row>
-    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="36" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="9">
         <f>SumEstJaneczek</f>
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="D6" s="18">
+        <v>0.125</v>
+      </c>
+      <c r="D6" s="38">
         <f>SumActJaneczek</f>
-        <v>1.113425925925926E-2</v>
+        <v>0.19831018518518517</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="9">
         <f>SumEstMair</f>
         <v>0</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="38">
         <f>SumActMair</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="40">
         <f>SUM(SumEstJaneczek+SumEstMair)</f>
-        <v>2.0833333333333332E-2</v>
-      </c>
-      <c r="D8" s="19">
+        <v>0.125</v>
+      </c>
+      <c r="D8" s="41">
         <f>SUM(SumActJaneczek+SumActMair)</f>
-        <v>1.113425925925926E-2</v>
+        <v>0.19831018518518517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>